<commit_message>
nothing to source, change students's infomation.
</commit_message>
<xml_diff>
--- a/gradefinal/studentsinfo.xlsx
+++ b/gradefinal/studentsinfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\docs\教学\2017-2018-2\毕业设计相关工作\成绩评定\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,6 +122,10 @@
   </si>
   <si>
     <t>答辩委员会评语</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该生毕业设计选题具有实际工程意义，设计质量良好，设计成果完整，具有较好的工程价值。答辩准备充分、称述问题清晰、回答问题良好。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -493,7 +497,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -552,13 +556,16 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="F2">
         <v>84</v>
       </c>
       <c r="G2">
         <v>80</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.25">
@@ -575,7 +582,7 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F3">
         <v>79</v>
@@ -621,13 +628,16 @@
         <v>17</v>
       </c>
       <c r="E5">
-        <v>70</v>
+        <v>81.3</v>
       </c>
       <c r="F5">
         <v>84</v>
       </c>
       <c r="G5">
         <v>80</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.25">
@@ -644,7 +654,7 @@
         <v>20</v>
       </c>
       <c r="E6">
-        <v>70</v>
+        <v>72.3</v>
       </c>
       <c r="F6">
         <v>80</v>
@@ -667,7 +677,7 @@
         <v>24</v>
       </c>
       <c r="E7">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F7">
         <v>73</v>

</xml_diff>